<commit_message>
ci: add TAS form
</commit_message>
<xml_diff>
--- a/LF/TAS/Cote d'Ivoire/Feb 2022/ci_lf_tas1_2_partcipants_202202.xlsx
+++ b/LF/TAS/Cote d'Ivoire/Feb 2022/ci_lf_tas1_2_partcipants_202202.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12345" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -339,10 +339,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Octobre 2021) 2. TAS1 FL - Formulaire Participants V3</t>
-  </si>
-  <si>
-    <t>ci_lf_tas1_2_partcipants_202110_v3</t>
+    <t>(February 2022) 2. TAS1 FL - Formulaire Participants</t>
+  </si>
+  <si>
+    <t>ci_lf_tas1_2_partcipants_202202</t>
   </si>
   <si>
     <t>French</t>
@@ -354,9 +354,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -401,6 +401,97 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -409,76 +500,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -492,13 +523,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,16 +531,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -529,24 +545,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -573,187 +573,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,6 +797,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -817,6 +832,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -870,175 +894,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1450,7 +1450,7 @@
   <sheetPr/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1458,26 +1458,26 @@
       <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.6266666666667" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="42.6266666666667" customWidth="1"/>
-    <col min="4" max="4" width="41.2533333333333" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="47.3733333333333" customWidth="1"/>
-    <col min="7" max="7" width="12.6266666666667" customWidth="1"/>
-    <col min="8" max="8" width="16.8733333333333" customWidth="1"/>
-    <col min="9" max="10" width="29.5" customWidth="1"/>
-    <col min="11" max="11" width="20.3733333333333" customWidth="1"/>
-    <col min="12" max="12" width="39.8733333333333" customWidth="1"/>
-    <col min="13" max="13" width="9.75333333333333" customWidth="1"/>
-    <col min="14" max="14" width="35.3733333333333" customWidth="1"/>
-    <col min="15" max="15" width="13.8733333333333" customWidth="1"/>
-    <col min="16" max="16" width="36.6266666666667" customWidth="1"/>
+    <col min="1" max="1" width="19.6296296296296" customWidth="1"/>
+    <col min="2" max="2" width="16.5037037037037" customWidth="1"/>
+    <col min="3" max="3" width="42.6296296296296" customWidth="1"/>
+    <col min="4" max="4" width="41.2518518518519" customWidth="1"/>
+    <col min="5" max="5" width="47.5037037037037" customWidth="1"/>
+    <col min="6" max="6" width="47.3703703703704" customWidth="1"/>
+    <col min="7" max="7" width="12.6296296296296" customWidth="1"/>
+    <col min="8" max="8" width="16.8740740740741" customWidth="1"/>
+    <col min="9" max="10" width="29.5037037037037" customWidth="1"/>
+    <col min="11" max="11" width="20.3703703703704" customWidth="1"/>
+    <col min="12" max="12" width="39.8740740740741" customWidth="1"/>
+    <col min="13" max="13" width="9.75555555555556" customWidth="1"/>
+    <col min="14" max="14" width="35.3703703703704" customWidth="1"/>
+    <col min="15" max="15" width="13.8740740740741" customWidth="1"/>
+    <col min="16" max="16" width="36.6296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="36" spans="1:16">
+    <row r="1" s="3" customFormat="1" ht="18" spans="1:16">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="63" spans="1:16">
+    <row r="2" s="3" customFormat="1" ht="57" spans="1:16">
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
@@ -1761,7 +1761,7 @@
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
     </row>
-    <row r="10" s="9" customFormat="1" customHeight="1" spans="1:16">
+    <row r="10" s="9" customFormat="1" ht="15.75" customHeight="1" spans="1:16">
       <c r="A10" s="17" t="s">
         <v>16</v>
       </c>
@@ -1797,7 +1797,7 @@
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
     </row>
-    <row r="11" s="3" customFormat="1" ht="31.5" spans="1:16">
+    <row r="11" s="3" customFormat="1" ht="28.5" spans="1:16">
       <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
@@ -1833,7 +1833,7 @@
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
     </row>
-    <row r="12" s="10" customFormat="1" ht="31.5" spans="1:16">
+    <row r="12" s="10" customFormat="1" ht="28.5" spans="1:16">
       <c r="A12" s="10" t="s">
         <v>16</v>
       </c>
@@ -1873,7 +1873,7 @@
       <c r="O12" s="19"/>
       <c r="P12" s="19"/>
     </row>
-    <row r="13" s="3" customFormat="1" ht="47.25" spans="1:16">
+    <row r="13" s="3" customFormat="1" ht="42.75" spans="1:16">
       <c r="A13" s="13" t="s">
         <v>26</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" s="3" customFormat="1" ht="31.5" spans="1:16">
+    <row r="14" s="3" customFormat="1" ht="28.5" spans="1:16">
       <c r="A14" s="13" t="s">
         <v>75</v>
       </c>
@@ -2017,18 +2017,18 @@
   <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.3733333333333" customWidth="1"/>
-    <col min="2" max="2" width="39.6266666666667" customWidth="1"/>
-    <col min="3" max="3" width="23.7533333333333" customWidth="1"/>
-    <col min="4" max="4" width="20.8733333333333" customWidth="1"/>
+    <col min="1" max="1" width="16.3703703703704" customWidth="1"/>
+    <col min="2" max="2" width="39.6296296296296" customWidth="1"/>
+    <col min="3" max="3" width="23.7555555555556" customWidth="1"/>
+    <col min="4" max="4" width="20.8740740740741" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2145,13 +2145,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="46.5" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="46.5037037037037" customWidth="1"/>
+    <col min="2" max="2" width="31.5037037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>